<commit_message>
Still dirty. Finished implementing pems loading
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_Results.xlsx
+++ b/xls/Cmaes_210E_Results.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenario" sheetId="4" r:id="rId1"/>
+    <sheet name="Settings" sheetId="4" r:id="rId1"/>
     <sheet name="cmaes" sheetId="1" r:id="rId2"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId4"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="74">
   <si>
     <t>Scenario</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>[1.405;0.68841]</t>
+  </si>
+  <si>
+    <t>[1.0417;0.8718]</t>
+  </si>
+  <si>
+    <t>210E</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Pems processed folder</t>
   </si>
 </sst>
 </file>
@@ -791,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,23 +814,36 @@
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -831,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AZ1" sqref="AZ1"/>
     </sheetView>
   </sheetViews>
@@ -952,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="AZ1" s="24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BA1" s="22"/>
       <c r="BB1" s="6"/>
@@ -3568,24 +3593,58 @@
       <c r="BB31" s="7"/>
     </row>
     <row r="32" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="7">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32" s="7">
+        <v>1500</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O32" s="7">
+        <v>0</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
+      <c r="R32" s="7">
+        <v>8</v>
+      </c>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>

</xml_diff>

<commit_message>
Remaining : connecting TVM constraint with algo
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_Results.xlsx
+++ b/xls/Cmaes_210E_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="77">
   <si>
     <t>Scenario</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Pems processed folder</t>
+  </si>
+  <si>
+    <t>[0;0]</t>
+  </si>
+  <si>
+    <t>[5;5]</t>
+  </si>
+  <si>
+    <t>[0.71394;1.8066]</t>
   </si>
 </sst>
 </file>
@@ -805,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -856,9 +865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AZ1" sqref="AZ1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +883,7 @@
     <col min="13" max="13" width="12" style="11" customWidth="1"/>
     <col min="14" max="14" width="18.5703125" style="11" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" style="11" customWidth="1"/>
     <col min="17" max="17" width="20" style="11" customWidth="1"/>
     <col min="18" max="18" width="18.5703125" style="11" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" style="9" customWidth="1"/>
@@ -977,7 +986,7 @@
         <v>26</v>
       </c>
       <c r="AZ1" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BA1" s="22"/>
       <c r="BB1" s="6"/>
@@ -3683,24 +3692,54 @@
       <c r="BB32" s="7"/>
     </row>
     <row r="33" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
+      <c r="H33" s="7">
+        <v>2</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="L33" s="7">
+        <v>1</v>
+      </c>
+      <c r="M33" s="7">
+        <v>1500</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O33" s="7">
+        <v>7767716647.3344612</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
+      <c r="R33" s="7">
+        <v>8</v>
+      </c>
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>

</xml_diff>

<commit_message>
Still trying to implement constraint.Code improved
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_Results.xlsx
+++ b/xls/Cmaes_210E_Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="82">
   <si>
     <t>Scenario</t>
   </si>
@@ -249,6 +249,21 @@
   </si>
   <si>
     <t>[0.71394;1.8066]</t>
+  </si>
+  <si>
+    <t>[1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25]</t>
+  </si>
+  <si>
+    <t>[0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5]</t>
+  </si>
+  <si>
+    <t>[0;0;0;0;0;0;0;0;0;0;0]</t>
+  </si>
+  <si>
+    <t>[2.6042;3.9683;5.2083;2.3981;1.3072;2.103;1.3072;1.3072;1.3072;1.3072;148.1481]</t>
+  </si>
+  <si>
+    <t>[2.1717;3.9683;1.8735;1.8476;0;1.9573;0;0.88062;0.53712;0.6878;12.4949]</t>
   </si>
 </sst>
 </file>
@@ -865,9 +880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AZ1" sqref="AZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +1001,7 @@
         <v>26</v>
       </c>
       <c r="AZ1" s="24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BA1" s="22"/>
       <c r="BB1" s="6"/>
@@ -3778,24 +3793,58 @@
       <c r="BB33" s="7"/>
     </row>
     <row r="34" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="7">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" s="7">
+        <v>1</v>
+      </c>
+      <c r="L34" s="7">
+        <v>1</v>
+      </c>
+      <c r="M34" s="7">
+        <v>1500</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O34" s="7">
+        <v>441898.12790347892</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
+      <c r="R34" s="7">
+        <v>13</v>
+      </c>
       <c r="S34" s="7"/>
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>

</xml_diff>

<commit_message>
Incremental improvements, added knobs rescaling
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_Results.xlsx
+++ b/xls/Cmaes_210E_Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="84">
   <si>
     <t>Scenario</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>[2.1717;3.9683;1.8735;1.8476;0;1.9573;0;0.88062;0.53712;0.6878;12.4949]</t>
+  </si>
+  <si>
+    <t>[2.3588;0.50392;4.7572;1.5164;0.1275;0.5857;0.71488;1.2516;1.2613;0.20603;143.7915]</t>
+  </si>
+  <si>
+    <t>[1.461;0.75774;5.2083;1.4052;0;0.28874;0.62948;0.93877;1.0628;0.22102;122.9023]</t>
   </si>
 </sst>
 </file>
@@ -880,9 +886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q38" sqref="Q38"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AZ1" sqref="AZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1007,7 @@
         <v>26</v>
       </c>
       <c r="AZ1" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="BA1" s="22"/>
       <c r="BB1" s="6"/>
@@ -3939,25 +3945,57 @@
       <c r="BB35" s="7"/>
     </row>
     <row r="36" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="H36" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I36" s="7">
+        <v>2</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L36" s="7">
+        <v>10</v>
+      </c>
+      <c r="M36" s="7">
+        <v>10</v>
+      </c>
+      <c r="N36" s="7">
+        <v>1000</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P36" s="7">
+        <v>5947954.8108171225</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
+      <c r="S36" s="7">
+        <v>13</v>
+      </c>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
       <c r="V36" s="7"/>

</xml_diff>